<commit_message>
Changed IRLZ44N for 2N7002
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnus/Developer/fifty-fifty/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E83E9AE-66EF-3849-B58E-27572D493C4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE4EE99-D5D1-7F41-8249-29BF9AB9E644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{155F3A06-4D17-5241-8AB7-237E1C0F671C}"/>
   </bookViews>
@@ -57,6 +57,9 @@
     <t>Mosfet</t>
   </si>
   <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
     <t>TSSOP-24_4.4x7.8x0.65P</t>
   </si>
   <si>
@@ -180,19 +183,16 @@
     <t>AVDD filter</t>
   </si>
   <si>
-    <t>IRLZ44NSTRLPBF</t>
-  </si>
-  <si>
-    <t>D2PAK</t>
-  </si>
-  <si>
-    <t>C538199</t>
-  </si>
-  <si>
     <t>ADS1232IPWR</t>
   </si>
   <si>
     <t>C27919</t>
+  </si>
+  <si>
+    <t>2N7002</t>
+  </si>
+  <si>
+    <t>C8545</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,10 +583,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -594,260 +594,260 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ref="C5:C10" si="0">"0402"</f>
         <v>0402</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="str">
         <f>"0402"</f>
         <v>0402</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ref="C12:C14" si="1">"0402"</f>
         <v>0402</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Final changes before ordering PCB
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnus/Developer/fifty-fifty/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE4EE99-D5D1-7F41-8249-29BF9AB9E644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9CCC37-63EF-7640-A0F8-AEE514FE0D4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{155F3A06-4D17-5241-8AB7-237E1C0F671C}"/>
+    <workbookView xWindow="19680" yWindow="880" windowWidth="33600" windowHeight="19160" xr2:uid="{155F3A06-4D17-5241-8AB7-237E1C0F671C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>Chip</t>
   </si>
@@ -117,12 +117,6 @@
     <t>R6</t>
   </si>
   <si>
-    <t>5V filter</t>
-  </si>
-  <si>
-    <t>GND filter</t>
-  </si>
-  <si>
     <t>AINP1 filter</t>
   </si>
   <si>
@@ -141,18 +135,9 @@
     <t>C4</t>
   </si>
   <si>
-    <t>10 nF</t>
-  </si>
-  <si>
     <t>100 nF</t>
   </si>
   <si>
-    <t>CL05B104KO5NNNC</t>
-  </si>
-  <si>
-    <t>C1525</t>
-  </si>
-  <si>
     <t>ADC cap</t>
   </si>
   <si>
@@ -162,12 +147,6 @@
     <t>REF filter</t>
   </si>
   <si>
-    <t>C15195</t>
-  </si>
-  <si>
-    <t>CL05B103KB5NNNC</t>
-  </si>
-  <si>
     <t>0402WGF510JTCE</t>
   </si>
   <si>
@@ -193,6 +172,63 @@
   </si>
   <si>
     <t>C8545</t>
+  </si>
+  <si>
+    <t>10 nF, C0G</t>
+  </si>
+  <si>
+    <t>100 nF, C0G</t>
+  </si>
+  <si>
+    <t>CGA3E2C0G1H103JT0Y0N</t>
+  </si>
+  <si>
+    <t>GRM31C5C1H104JA01L</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>XC6206P502MR</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>SSR bleed</t>
+  </si>
+  <si>
+    <t>REFP filter</t>
+  </si>
+  <si>
+    <t>REFN filter</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>DVDD filter</t>
+  </si>
+  <si>
+    <t>C16767</t>
+  </si>
+  <si>
+    <t>C76710</t>
+  </si>
+  <si>
+    <t>C97946</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>LDO VI</t>
+  </si>
+  <si>
+    <t>LDO VO</t>
   </si>
 </sst>
 </file>
@@ -558,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D47EAA-CA8B-444C-AFCE-C43C28AAAA00}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -603,12 +639,12 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -617,87 +653,86 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" ref="C5:C10" si="0">"0402"</f>
-        <v>0402</v>
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C6:C11" si="0">"0402"</f>
         <v>0402</v>
       </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -705,20 +740,20 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
@@ -726,20 +761,20 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -747,20 +782,20 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -768,90 +803,174 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C11" t="str">
-        <f>"0402"</f>
+        <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" ref="C12:C14" si="1">"0402"</f>
-        <v>0402</v>
+        <f>"0603"</f>
+        <v>0603</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>0402</v>
+        <f>"0603"</f>
+        <v>0603</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="str">
+        <f>"1206"</f>
+        <v>1206</v>
+      </c>
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>0402</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" s="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="str">
+        <f>"1206"</f>
+        <v>1206</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="str">
+        <f>"1206"</f>
+        <v>1206</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="str">
+        <f>"1206"</f>
+        <v>1206</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="str">
+        <f>"1206"</f>
+        <v>1206</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Updated to revision C PCB
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnus/Developer/fifty-fifty/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9CCC37-63EF-7640-A0F8-AEE514FE0D4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6089CB62-D512-8546-9C9C-6F19ED2A101D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19680" yWindow="880" windowWidth="33600" windowHeight="19160" xr2:uid="{155F3A06-4D17-5241-8AB7-237E1C0F671C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{155F3A06-4D17-5241-8AB7-237E1C0F671C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Chip</t>
   </si>
@@ -114,9 +114,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>AINP1 filter</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
   </si>
   <si>
     <t>LDO</t>
-  </si>
-  <si>
-    <t>SSR bleed</t>
   </si>
   <si>
     <t>REFP filter</t>
@@ -594,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D47EAA-CA8B-444C-AFCE-C43C28AAAA00}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -639,24 +633,24 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -664,7 +658,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -673,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -701,17 +695,17 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:C11" si="0">"0402"</f>
+        <f t="shared" ref="C6:C10" si="0">"0402"</f>
         <v>0402</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -722,17 +716,17 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -743,17 +737,17 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
@@ -764,17 +758,17 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>0402</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -785,7 +779,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -795,7 +789,7 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -803,23 +797,23 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>0402</v>
+        <f>"0603"</f>
+        <v>0603</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -827,20 +821,20 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" t="str">
         <f>"0603"</f>
         <v>0603</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -851,14 +845,14 @@
         <v>48</v>
       </c>
       <c r="C13" t="str">
-        <f>"0603"</f>
-        <v>0603</v>
+        <f>"1206"</f>
+        <v>1206</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
         <v>46</v>
@@ -869,108 +863,87 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" t="str">
         <f>"1206"</f>
         <v>1206</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" t="str">
         <f>"1206"</f>
         <v>1206</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="str">
         <f>"1206"</f>
         <v>1206</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="str">
         <f>"1206"</f>
         <v>1206</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="str">
-        <f>"1206"</f>
-        <v>1206</v>
-      </c>
-      <c r="D18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="1"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>